<commit_message>
Edit TC verify Display the news function
</commit_message>
<xml_diff>
--- a/RecruitmentCMCAutoTest/NewsData.xlsx
+++ b/RecruitmentCMCAutoTest/NewsData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>id</t>
   </si>
@@ -42,9 +42,6 @@
     <t>detailContent</t>
   </si>
   <si>
-    <t>4 ƯU TIÊN CỦA CFO TRONG NĂM 2020 CHO NỀN TẢNG TÀI CHÍNH DOANH NGHIỆP VỮNG CHẮC</t>
-  </si>
-  <si>
     <t>Trong năm 2020, trước tình hình thực tế</t>
   </si>
   <si>
@@ -63,118 +60,43 @@
     <t>1587355164029.png</t>
   </si>
   <si>
+    <t>Trung bình, mỗi người ở độ tuổi đi làm dành 1/3 thời gian trong ngày để dành cho công việc</t>
+  </si>
+  <si>
+    <t>06-08-2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 22-08-2018</t>
+  </si>
+  <si>
+    <t>Sau 1 khoảng thời gian thử thách, cuối cùng bạn cũng nhận được cú điện thoại mời đến văn phòng phỏng vấn của nhà tuyển dụng.</t>
+  </si>
+  <si>
+    <t>Đây là câu hỏi mở đầu của mọi buổi phỏng vấn</t>
+  </si>
+  <si>
+    <t>1534934239126.png</t>
+  </si>
+  <si>
+    <t>HỠI ỨNG VIÊN QUỐC DÂN! CHÚNG TÔI KHÔNG CÓ CẢ NGÀY CHỈ ĐỂ CHỜ ĐỢI BẠN!</t>
+  </si>
+  <si>
+    <t>Lướt dọc, xẻ ngang các trang báo mạng, các nhóm cộng đồng trên mạng xã hội</t>
+  </si>
+  <si>
+    <t>Không riêng một ai, một trong những phản ứng chung nhất của mọi ứng viên khi nhận được cuộc gọi mời đi phỏng vấn</t>
+  </si>
+  <si>
+    <t>22-08-2018</t>
+  </si>
+  <si>
+    <t>1534933313486.png</t>
+  </si>
+  <si>
     <t>5 CÂU HỎI PHỎNG VẤN “TOÁT MỒ HÔI” KINH ĐIỂN CỦA NHÀ TUYỂN DỤNG</t>
   </si>
   <si>
-    <t>Trung bình, mỗi người ở độ tuổi đi làm dành 1/3 thời gian trong ngày để dành cho công việc</t>
-  </si>
-  <si>
-    <t>06-08-2019</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 22-08-2018</t>
-  </si>
-  <si>
-    <t>Sau 1 khoảng thời gian thử thách, cuối cùng bạn cũng nhận được cú điện thoại mời đến văn phòng phỏng vấn của nhà tuyển dụng.</t>
-  </si>
-  <si>
-    <t>Đây là câu hỏi mở đầu của mọi buổi phỏng vấn</t>
-  </si>
-  <si>
-    <t>1534934239126.png</t>
-  </si>
-  <si>
-    <t>HỠI ỨNG VIÊN QUỐC DÂN! CHÚNG TÔI KHÔNG CÓ CẢ NGÀY CHỈ ĐỂ CHỜ ĐỢI BẠN!</t>
-  </si>
-  <si>
-    <t>Lướt dọc, xẻ ngang các trang báo mạng, các nhóm cộng đồng trên mạng xã hội</t>
-  </si>
-  <si>
-    <t>Không riêng một ai, một trong những phản ứng chung nhất của mọi ứng viên khi nhận được cuộc gọi mời đi phỏng vấn</t>
-  </si>
-  <si>
-    <t>22-08-2018</t>
-  </si>
-  <si>
-    <t>1534933313486.png</t>
-  </si>
-  <si>
-    <t>LÀM THẾ NÀO ĐỂ THUỘC NHÓM 8% NGƯỜI LUÔN ĐẠT ĐƯỢC MỤC TIÊU?</t>
-  </si>
-  <si>
-    <t>Theo các nghiên cứu, có tới 92% lượng người không bao giờ đạt được mục tiêu do chính bản thân đề ra</t>
-  </si>
-  <si>
-    <t>Nhà tâm lý học Angela Duckworth tin rằng yếu tố nổi bật giúp người thành công đạt được mục tiêu của mình là khả năng vượt qua thất bại và tự phục hồi nhanh chóng</t>
-  </si>
-  <si>
-    <t>1534932775136.png</t>
-  </si>
-  <si>
-    <t>50 MẸO GIÚP TĂNG HIỆU SUẤT CÔNG VIỆC</t>
-  </si>
-  <si>
-    <t>Để tăng hiệu suất công việc, bạn cần cải thiện các yếu tố cơ bản như khả năng tập trung</t>
-  </si>
-  <si>
-    <t>1534931747829.png</t>
-  </si>
-  <si>
-    <t>NHỮNG NIỀM ĐAU CHÔN GIẤU CỦA NHÀ TUYỂN DỤNG KHI ĐỌC CV</t>
-  </si>
-  <si>
-    <t>Bạn biết không, nếu ứng viên cứ phải băn khoăn chẳng biết cách nào để CV của mình “lọt vào mắt xanh” của nhà tuyển dụng</t>
-  </si>
-  <si>
-    <t>Tất tần tật những vấn đề như sai chính tả, sai ngữ pháp, viết sai tên công ty,…là những chuyện không thể chấp nhận được</t>
-  </si>
-  <si>
-    <t>1534931143304.png</t>
-  </si>
-  <si>
-    <t>NHỮNG LỖI EMAIL TAI HẠI KHIẾN BẠN CHẲNG BAO GIỜ ĐƯỢC HẸN PHỎNG VẤN</t>
-  </si>
-  <si>
-    <t>Bạn có bao giờ tự hỏi tại sao mình ứng tuyển rất nhiều rồi mà không bao giờ thấy công ty hẹn đi phỏng vấn?</t>
-  </si>
-  <si>
-    <t>Việc này có thể tiết kiệm thời gian của bạn đôi chút nhưng vô tình khiến cho hồ sơ của bạn bị lãng quên không thương tiếc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22-08-2018 </t>
-  </si>
-  <si>
-    <t>1534930771044.png</t>
-  </si>
-  <si>
-    <t>CÁCH VƯỢT QUA NHỮNG CÂU HỎI “TƯỞNG KHÔNG KHÓ MÀ KHÓ KHÔNG TƯỞNG” KHI PHỎNG VẤN</t>
-  </si>
-  <si>
-    <t>Khi phỏng vấn xin việc, ở khâu chuẩn bị, dường như các ứng viên chỉ tập trung tìm kiếm</t>
-  </si>
-  <si>
-    <t>1534930542180.png</t>
-  </si>
-  <si>
-    <t>Không đơn thuần là giới thiệu những thông tin cá nhân cơ bản vì chắc chắn nhà tuyển dụng đã “nghiên cứu” rất kĩ CV</t>
-  </si>
-  <si>
-    <t>22-08-2019</t>
-  </si>
-  <si>
-    <t>EM “GIẬN” CÔNG TY ĐÃ TỪ CHỐI TUYỂN EM, CÓ HỢP LÝ KHÔNG?</t>
-  </si>
-  <si>
-    <t>Hôm nay em vô tình xem lại email của phòng nhân sự nọ gửi cho mình nên nhớ lại sự việc này</t>
-  </si>
-  <si>
-    <t>21-08-2018</t>
-  </si>
-  <si>
-    <t>1534914208705.png</t>
-  </si>
-  <si>
-    <t>Em nghĩ họ cũng nên xin lỗi em một tiếng vì em cũng đã đến làm bài test và phỏng vấn đến 2 buổi</t>
+    <t>4 ƯU TIÊN CỦA CFO TRONG NĂM 2020 CHO NỀN TẢNG TÀI CHÍNH DOANH NGHIỆP VỮNG CHẮC AAAAAAAAAAAA</t>
   </si>
 </sst>
 </file>
@@ -512,16 +434,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.42578125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="31.42578125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="38.7109375" style="2" customWidth="1"/>
     <col min="3" max="3" width="28.28515625" style="2" customWidth="1"/>
     <col min="4" max="4" width="28" style="2" customWidth="1"/>
     <col min="5" max="5" width="36.85546875" style="2" customWidth="1"/>
@@ -554,16 +476,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>9</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>5</v>
@@ -574,39 +496,39 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="E3" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -614,136 +536,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="2" t="s">
+      <c r="F5" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>7</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>8</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <v>9</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
-        <v>10</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Edit TC verify Like function & display the news
</commit_message>
<xml_diff>
--- a/RecruitmentCMCAutoTest/NewsData.xlsx
+++ b/RecruitmentCMCAutoTest/NewsData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>id</t>
   </si>
@@ -42,9 +42,6 @@
     <t>detailContent</t>
   </si>
   <si>
-    <t>4 ƯU TIÊN CỦA CFO TRONG NĂM 2020 CHO NỀN TẢNG TÀI CHÍNH DOANH NGHIỆP VỮNG CHẮC</t>
-  </si>
-  <si>
     <t>Trong năm 2020, trước tình hình thực tế</t>
   </si>
   <si>
@@ -99,82 +96,7 @@
     <t>1534933313486.png</t>
   </si>
   <si>
-    <t>LÀM THẾ NÀO ĐỂ THUỘC NHÓM 8% NGƯỜI LUÔN ĐẠT ĐƯỢC MỤC TIÊU?</t>
-  </si>
-  <si>
-    <t>Theo các nghiên cứu, có tới 92% lượng người không bao giờ đạt được mục tiêu do chính bản thân đề ra</t>
-  </si>
-  <si>
-    <t>Nhà tâm lý học Angela Duckworth tin rằng yếu tố nổi bật giúp người thành công đạt được mục tiêu của mình là khả năng vượt qua thất bại và tự phục hồi nhanh chóng</t>
-  </si>
-  <si>
-    <t>1534932775136.png</t>
-  </si>
-  <si>
-    <t>50 MẸO GIÚP TĂNG HIỆU SUẤT CÔNG VIỆC</t>
-  </si>
-  <si>
-    <t>Để tăng hiệu suất công việc, bạn cần cải thiện các yếu tố cơ bản như khả năng tập trung</t>
-  </si>
-  <si>
-    <t>1534931747829.png</t>
-  </si>
-  <si>
-    <t>NHỮNG NIỀM ĐAU CHÔN GIẤU CỦA NHÀ TUYỂN DỤNG KHI ĐỌC CV</t>
-  </si>
-  <si>
-    <t>Bạn biết không, nếu ứng viên cứ phải băn khoăn chẳng biết cách nào để CV của mình “lọt vào mắt xanh” của nhà tuyển dụng</t>
-  </si>
-  <si>
-    <t>Tất tần tật những vấn đề như sai chính tả, sai ngữ pháp, viết sai tên công ty,…là những chuyện không thể chấp nhận được</t>
-  </si>
-  <si>
-    <t>1534931143304.png</t>
-  </si>
-  <si>
-    <t>NHỮNG LỖI EMAIL TAI HẠI KHIẾN BẠN CHẲNG BAO GIỜ ĐƯỢC HẸN PHỎNG VẤN</t>
-  </si>
-  <si>
-    <t>Bạn có bao giờ tự hỏi tại sao mình ứng tuyển rất nhiều rồi mà không bao giờ thấy công ty hẹn đi phỏng vấn?</t>
-  </si>
-  <si>
-    <t>Việc này có thể tiết kiệm thời gian của bạn đôi chút nhưng vô tình khiến cho hồ sơ của bạn bị lãng quên không thương tiếc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22-08-2018 </t>
-  </si>
-  <si>
-    <t>1534930771044.png</t>
-  </si>
-  <si>
-    <t>CÁCH VƯỢT QUA NHỮNG CÂU HỎI “TƯỞNG KHÔNG KHÓ MÀ KHÓ KHÔNG TƯỞNG” KHI PHỎNG VẤN</t>
-  </si>
-  <si>
-    <t>Khi phỏng vấn xin việc, ở khâu chuẩn bị, dường như các ứng viên chỉ tập trung tìm kiếm</t>
-  </si>
-  <si>
-    <t>1534930542180.png</t>
-  </si>
-  <si>
-    <t>Không đơn thuần là giới thiệu những thông tin cá nhân cơ bản vì chắc chắn nhà tuyển dụng đã “nghiên cứu” rất kĩ CV</t>
-  </si>
-  <si>
-    <t>22-08-2019</t>
-  </si>
-  <si>
-    <t>EM “GIẬN” CÔNG TY ĐÃ TỪ CHỐI TUYỂN EM, CÓ HỢP LÝ KHÔNG?</t>
-  </si>
-  <si>
-    <t>Hôm nay em vô tình xem lại email của phòng nhân sự nọ gửi cho mình nên nhớ lại sự việc này</t>
-  </si>
-  <si>
-    <t>21-08-2018</t>
-  </si>
-  <si>
-    <t>1534914208705.png</t>
-  </si>
-  <si>
-    <t>Em nghĩ họ cũng nên xin lỗi em một tiếng vì em cũng đã đến làm bài test và phỏng vấn đến 2 buổi</t>
+    <t>4 ƯU TIÊN CỦA CFO TRONG NĂM 2020 CHO NỀN TẢNG TÀI CHÍNH DOANH NGHIỆP VỮNG CHẮC  aaaaa</t>
   </si>
 </sst>
 </file>
@@ -512,16 +434,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.42578125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="31.42578125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="40" style="2" customWidth="1"/>
     <col min="3" max="3" width="28.28515625" style="2" customWidth="1"/>
     <col min="4" max="4" width="28" style="2" customWidth="1"/>
     <col min="5" max="5" width="36.85546875" style="2" customWidth="1"/>
@@ -554,16 +476,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>9</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>5</v>
@@ -574,19 +496,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="E3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="75" x14ac:dyDescent="0.25">
@@ -594,19 +516,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="F4" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -614,136 +536,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>7</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>8</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <v>9</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
-        <v>10</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Edit TC like function
</commit_message>
<xml_diff>
--- a/RecruitmentCMCAutoTest/NewsData.xlsx
+++ b/RecruitmentCMCAutoTest/NewsData.xlsx
@@ -96,7 +96,7 @@
     <t>5 CÂU HỎI PHỎNG VẤN “TOÁT MỒ HÔI” KINH ĐIỂN CỦA NHÀ TUYỂN DỤNG</t>
   </si>
   <si>
-    <t>4 ƯU TIÊN CỦA CFO TRONG NĂM 2020 CHO NỀN TẢNG TÀI CHÍNH DOANH NGHIỆP VỮNG CHẮC AAAAAAAAAAAA</t>
+    <t>4 ƯU TIÊN CỦA CFO TRONG NĂM 2020 CHO NỀN TẢNG TÀI CHÍNH DOANH NGHIỆP VỮNG CHẮC</t>
   </si>
 </sst>
 </file>
@@ -437,7 +437,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>